<commit_message>
speedup with lookup tables pt2
</commit_message>
<xml_diff>
--- a/Hi.xlsx
+++ b/Hi.xlsx
@@ -606,7 +606,7 @@
         <v>2</v>
       </c>
       <c r="J2" t="n">
-        <v>28.40163423767804</v>
+        <v>27.99187006961076</v>
       </c>
       <c r="K2" t="n">
         <v>0.4</v>
@@ -664,10 +664,10 @@
         <v>100</v>
       </c>
       <c r="AB2" t="n">
-        <v>28.40163423767804</v>
+        <v>27.99187006961076</v>
       </c>
       <c r="AC2" t="n">
-        <v>22.72976175065906</v>
+        <v>27.99187006961076</v>
       </c>
     </row>
     <row r="3">
@@ -701,7 +701,7 @@
         <v>4</v>
       </c>
       <c r="J3" t="n">
-        <v>28.04482673002215</v>
+        <v>27.60218805472812</v>
       </c>
       <c r="K3" t="n">
         <v>0.4</v>
@@ -759,10 +759,10 @@
         <v>100</v>
       </c>
       <c r="AB3" t="n">
-        <v>28.04482673002215</v>
+        <v>27.60218805472812</v>
       </c>
       <c r="AC3" t="n">
-        <v>21.6922617268172</v>
+        <v>27.60218805472812</v>
       </c>
     </row>
     <row r="4">
@@ -796,7 +796,7 @@
         <v>8</v>
       </c>
       <c r="J4" t="n">
-        <v>28.00425289934985</v>
+        <v>27.54465938100303</v>
       </c>
       <c r="K4" t="n">
         <v>0.4</v>
@@ -854,10 +854,10 @@
         <v>100</v>
       </c>
       <c r="AB4" t="n">
-        <v>28.00425289934985</v>
+        <v>27.54465938100303</v>
       </c>
       <c r="AC4" t="n">
-        <v>21.17351171489627</v>
+        <v>27.54465938100303</v>
       </c>
     </row>
     <row r="5">
@@ -891,7 +891,7 @@
         <v>2</v>
       </c>
       <c r="J5" t="n">
-        <v>26.30178224318103</v>
+        <v>25.81421241681556</v>
       </c>
       <c r="K5" t="n">
         <v>0.4</v>
@@ -949,10 +949,10 @@
         <v>100</v>
       </c>
       <c r="AB5" t="n">
-        <v>26.30178224318103</v>
+        <v>25.81421241681556</v>
       </c>
       <c r="AC5" t="n">
-        <v>18.01785694107058</v>
+        <v>25.81421241681556</v>
       </c>
     </row>
     <row r="6">
@@ -986,7 +986,7 @@
         <v>4</v>
       </c>
       <c r="J6" t="n">
-        <v>25.90208379764785</v>
+        <v>25.38710696946947</v>
       </c>
       <c r="K6" t="n">
         <v>0.4</v>
@@ -1044,10 +1044,10 @@
         <v>100</v>
       </c>
       <c r="AB6" t="n">
-        <v>25.90208379764785</v>
+        <v>25.38710696946947</v>
       </c>
       <c r="AC6" t="n">
-        <v>16.95535694107058</v>
+        <v>25.38710696946947</v>
       </c>
     </row>
     <row r="7">
@@ -1081,7 +1081,7 @@
         <v>8</v>
       </c>
       <c r="J7" t="n">
-        <v>25.8388455761803</v>
+        <v>25.30950471977179</v>
       </c>
       <c r="K7" t="n">
         <v>0.4</v>
@@ -1139,10 +1139,10 @@
         <v>100</v>
       </c>
       <c r="AB7" t="n">
-        <v>25.8388455761803</v>
+        <v>25.30950471977179</v>
       </c>
       <c r="AC7" t="n">
-        <v>16.42410694107058</v>
+        <v>25.30950471977179</v>
       </c>
     </row>
     <row r="8">
@@ -1176,7 +1176,7 @@
         <v>2</v>
       </c>
       <c r="J8" t="n">
-        <v>25.36582878501567</v>
+        <v>24.82388561306556</v>
       </c>
       <c r="K8" t="n">
         <v>0.4</v>
@@ -1234,10 +1234,10 @@
         <v>100</v>
       </c>
       <c r="AB8" t="n">
-        <v>25.36582878501567</v>
+        <v>24.82388561306556</v>
       </c>
       <c r="AC8" t="n">
-        <v>16.02704056685625</v>
+        <v>24.82388561306556</v>
       </c>
     </row>
     <row r="9">
@@ -1271,7 +1271,7 @@
         <v>4</v>
       </c>
       <c r="J9" t="n">
-        <v>24.93599700478827</v>
+        <v>24.37519151106132</v>
       </c>
       <c r="K9" t="n">
         <v>0.4</v>
@@ -1329,10 +1329,10 @@
         <v>100</v>
       </c>
       <c r="AB9" t="n">
-        <v>24.93599700478827</v>
+        <v>24.37519151106132</v>
       </c>
       <c r="AC9" t="n">
-        <v>14.93954059069811</v>
+        <v>24.37519151106132</v>
       </c>
     </row>
     <row r="10">
@@ -1366,7 +1366,7 @@
         <v>8</v>
       </c>
       <c r="J10" t="n">
-        <v>24.85680201510686</v>
+        <v>24.28592585215918</v>
       </c>
       <c r="K10" t="n">
         <v>0.4</v>
@@ -1424,10 +1424,10 @@
         <v>100</v>
       </c>
       <c r="AB10" t="n">
-        <v>24.85680201510686</v>
+        <v>24.28592585215918</v>
       </c>
       <c r="AC10" t="n">
-        <v>14.39579060261904</v>
+        <v>24.28592585215918</v>
       </c>
     </row>
     <row r="11">
@@ -1461,7 +1461,7 @@
         <v>2</v>
       </c>
       <c r="J11" t="n">
-        <v>19.87476135780198</v>
+        <v>19.74970716676716</v>
       </c>
       <c r="K11" t="n">
         <v>0.4</v>
@@ -1519,10 +1519,10 @@
         <v>100</v>
       </c>
       <c r="AB11" t="n">
-        <v>19.87476135780198</v>
+        <v>19.74970716676716</v>
       </c>
       <c r="AC11" t="n">
-        <v>16.89642837075961</v>
+        <v>19.74970716676716</v>
       </c>
     </row>
     <row r="12">
@@ -1556,7 +1556,7 @@
         <v>4</v>
       </c>
       <c r="J12" t="n">
-        <v>19.46611210661129</v>
+        <v>19.31177628505161</v>
       </c>
       <c r="K12" t="n">
         <v>0.4</v>
@@ -1614,10 +1614,10 @@
         <v>100</v>
       </c>
       <c r="AB12" t="n">
-        <v>19.46611210661129</v>
+        <v>19.31177628505161</v>
       </c>
       <c r="AC12" t="n">
-        <v>15.85892834691775</v>
+        <v>19.31177628505161</v>
       </c>
     </row>
     <row r="13">
@@ -1651,7 +1651,7 @@
         <v>8</v>
       </c>
       <c r="J13" t="n">
-        <v>19.39786668479999</v>
+        <v>19.22833286994427</v>
       </c>
       <c r="K13" t="n">
         <v>0.4</v>
@@ -1709,10 +1709,10 @@
         <v>100</v>
       </c>
       <c r="AB13" t="n">
-        <v>19.39786668479999</v>
+        <v>19.22833286994427</v>
       </c>
       <c r="AC13" t="n">
-        <v>15.34017833499682</v>
+        <v>19.22833286994427</v>
       </c>
     </row>
     <row r="14">
@@ -1746,7 +1746,7 @@
         <v>2</v>
       </c>
       <c r="J14" t="n">
-        <v>17.49667468712789</v>
+        <v>17.32040946817778</v>
       </c>
       <c r="K14" t="n">
         <v>0.4</v>
@@ -1804,10 +1804,10 @@
         <v>100</v>
       </c>
       <c r="AB14" t="n">
-        <v>17.49667468712789</v>
+        <v>17.32040946817778</v>
       </c>
       <c r="AC14" t="n">
-        <v>12.18452356117113</v>
+        <v>17.32040946817778</v>
       </c>
     </row>
     <row r="15">
@@ -1841,7 +1841,7 @@
         <v>4</v>
       </c>
       <c r="J15" t="n">
-        <v>17.01577394474345</v>
+        <v>16.81784124483682</v>
       </c>
       <c r="K15" t="n">
         <v>0.4</v>
@@ -1899,10 +1899,10 @@
         <v>100</v>
       </c>
       <c r="AB15" t="n">
-        <v>17.01577394474345</v>
+        <v>16.81784124483682</v>
       </c>
       <c r="AC15" t="n">
-        <v>11.12202356117113</v>
+        <v>16.81784124483682</v>
       </c>
     </row>
     <row r="16">
@@ -1936,7 +1936,7 @@
         <v>8</v>
       </c>
       <c r="J16" t="n">
-        <v>16.90864044175108</v>
+        <v>16.69922881674465</v>
       </c>
       <c r="K16" t="n">
         <v>0.4</v>
@@ -1994,10 +1994,10 @@
         <v>100</v>
       </c>
       <c r="AB16" t="n">
-        <v>16.90864044175108</v>
+        <v>16.69922881674465</v>
       </c>
       <c r="AC16" t="n">
-        <v>10.59077356117113</v>
+        <v>16.69922881674465</v>
       </c>
     </row>
     <row r="17">
@@ -2031,7 +2031,7 @@
         <v>2</v>
       </c>
       <c r="J17" t="n">
-        <v>16.40124830478942</v>
+        <v>16.18113487099227</v>
       </c>
       <c r="K17" t="n">
         <v>0.4</v>
@@ -2089,10 +2089,10 @@
         <v>100</v>
       </c>
       <c r="AB17" t="n">
-        <v>16.40124830478942</v>
+        <v>16.18113487099227</v>
       </c>
       <c r="AC17" t="n">
-        <v>10.1937071869568</v>
+        <v>16.18113487099227</v>
       </c>
     </row>
     <row r="18">
@@ -2126,7 +2126,7 @@
         <v>4</v>
       </c>
       <c r="J18" t="n">
-        <v>15.86973002469453</v>
+        <v>15.63892530632404</v>
       </c>
       <c r="K18" t="n">
         <v>0.4</v>
@@ -2184,10 +2184,10 @@
         <v>100</v>
       </c>
       <c r="AB18" t="n">
-        <v>15.86973002469453</v>
+        <v>15.63892530632404</v>
       </c>
       <c r="AC18" t="n">
-        <v>9.106207210798662</v>
+        <v>15.63892530632404</v>
       </c>
     </row>
     <row r="19">
@@ -2221,7 +2221,7 @@
         <v>8</v>
       </c>
       <c r="J19" t="n">
-        <v>15.73513302640055</v>
+        <v>15.49851661728377</v>
       </c>
       <c r="K19" t="n">
         <v>0.4</v>
@@ -2279,10 +2279,10 @@
         <v>100</v>
       </c>
       <c r="AB19" t="n">
-        <v>15.73513302640055</v>
+        <v>15.49851661728377</v>
       </c>
       <c r="AC19" t="n">
-        <v>8.562457222719591</v>
+        <v>15.49851661728377</v>
       </c>
     </row>
     <row r="20">
@@ -2316,7 +2316,7 @@
         <v>2</v>
       </c>
       <c r="J20" t="n">
-        <v>17.68310497397308</v>
+        <v>17.64592457541496</v>
       </c>
       <c r="K20" t="n">
         <v>0.4</v>
@@ -2374,10 +2374,10 @@
         <v>100</v>
       </c>
       <c r="AB20" t="n">
-        <v>17.68310497397308</v>
+        <v>17.64592457541496</v>
       </c>
       <c r="AC20" t="n">
-        <v>15.43809516160262</v>
+        <v>17.64592457541496</v>
       </c>
     </row>
     <row r="21">
@@ -2411,7 +2411,7 @@
         <v>4</v>
       </c>
       <c r="J21" t="n">
-        <v>17.2559133529331</v>
+        <v>17.19137496712583</v>
       </c>
       <c r="K21" t="n">
         <v>0.4</v>
@@ -2469,10 +2469,10 @@
         <v>100</v>
       </c>
       <c r="AB21" t="n">
-        <v>17.2559133529331</v>
+        <v>17.19137496712583</v>
       </c>
       <c r="AC21" t="n">
-        <v>14.40059513776076</v>
+        <v>17.19137496712583</v>
       </c>
     </row>
     <row r="22">
@@ -2506,7 +2506,7 @@
         <v>8</v>
       </c>
       <c r="J22" t="n">
-        <v>17.17769188719105</v>
+        <v>17.09893612708201</v>
       </c>
       <c r="K22" t="n">
         <v>0.4</v>
@@ -2564,10 +2564,10 @@
         <v>100</v>
       </c>
       <c r="AB22" t="n">
-        <v>17.17769188719105</v>
+        <v>17.09893612708201</v>
       </c>
       <c r="AC22" t="n">
-        <v>13.88184512583983</v>
+        <v>17.09893612708201</v>
       </c>
     </row>
     <row r="23">
@@ -2601,7 +2601,7 @@
         <v>2</v>
       </c>
       <c r="J23" t="n">
-        <v>15.20328873852896</v>
+        <v>15.12814465154436</v>
       </c>
       <c r="K23" t="n">
         <v>0.4</v>
@@ -2659,10 +2659,10 @@
         <v>100</v>
       </c>
       <c r="AB23" t="n">
-        <v>15.20328873852896</v>
+        <v>15.12814465154436</v>
       </c>
       <c r="AC23" t="n">
-        <v>10.72619035201414</v>
+        <v>15.12814465154436</v>
       </c>
     </row>
     <row r="24">
@@ -2696,7 +2696,7 @@
         <v>4</v>
       </c>
       <c r="J24" t="n">
-        <v>14.69169892390044</v>
+        <v>14.59819771446141</v>
       </c>
       <c r="K24" t="n">
         <v>0.4</v>
@@ -2754,10 +2754,10 @@
         <v>100</v>
       </c>
       <c r="AB24" t="n">
-        <v>14.69169892390044</v>
+        <v>14.59819771446141</v>
       </c>
       <c r="AC24" t="n">
-        <v>9.663690352014138</v>
+        <v>14.59819771446141</v>
       </c>
     </row>
     <row r="25">
@@ -2791,7 +2791,7 @@
         <v>8</v>
       </c>
       <c r="J25" t="n">
-        <v>14.56779342568837</v>
+        <v>14.4645490643557</v>
       </c>
       <c r="K25" t="n">
         <v>0.4</v>
@@ -2849,10 +2849,10 @@
         <v>100</v>
       </c>
       <c r="AB25" t="n">
-        <v>14.56779342568837</v>
+        <v>14.4645490643557</v>
       </c>
       <c r="AC25" t="n">
-        <v>9.132440352014138</v>
+        <v>14.4645490643557</v>
       </c>
     </row>
     <row r="26">
@@ -2886,7 +2886,7 @@
         <v>2</v>
       </c>
       <c r="J26" t="n">
-        <v>14.04717827249717</v>
+        <v>13.93447080663309</v>
       </c>
       <c r="K26" t="n">
         <v>0.4</v>
@@ -2944,10 +2944,10 @@
         <v>100</v>
       </c>
       <c r="AB26" t="n">
-        <v>14.04717827249717</v>
+        <v>13.93447080663309</v>
       </c>
       <c r="AC26" t="n">
-        <v>8.73537397779981</v>
+        <v>13.93447080663309</v>
       </c>
     </row>
     <row r="27">
@@ -2981,7 +2981,7 @@
         <v>4</v>
       </c>
       <c r="J27" t="n">
-        <v>13.47609444897525</v>
+        <v>13.35737332032622</v>
       </c>
       <c r="K27" t="n">
         <v>0.4</v>
@@ -3039,10 +3039,10 @@
         <v>100</v>
       </c>
       <c r="AB27" t="n">
-        <v>13.47609444897525</v>
+        <v>13.35737332032622</v>
       </c>
       <c r="AC27" t="n">
-        <v>7.647874001641668</v>
+        <v>13.35737332032622</v>
       </c>
     </row>
     <row r="28">
@@ -3076,7 +3076,7 @@
         <v>8</v>
       </c>
       <c r="J28" t="n">
-        <v>13.31966070824493</v>
+        <v>13.19765080018907</v>
       </c>
       <c r="K28" t="n">
         <v>0.4</v>
@@ -3134,10 +3134,10 @@
         <v>100</v>
       </c>
       <c r="AB28" t="n">
-        <v>13.31966070824493</v>
+        <v>13.19765080018907</v>
       </c>
       <c r="AC28" t="n">
-        <v>7.104124013562597</v>
+        <v>13.19765080018907</v>
       </c>
     </row>
   </sheetData>

</xml_diff>